<commit_message>
Updated after migrating objects.
</commit_message>
<xml_diff>
--- a/Customer/Elas/Object Migrate Overview.xlsx
+++ b/Customer/Elas/Object Migrate Overview.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="1130">
   <si>
     <t>Type</t>
   </si>
@@ -3401,13 +3401,34 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>Client Monitor</t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>Target only</t>
+  </si>
+  <si>
+    <t>Not merged</t>
+  </si>
+  <si>
+    <t>Will be deleted</t>
+  </si>
+  <si>
+    <t>System table</t>
+  </si>
+  <si>
+    <t>Nota actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3419,6 +3440,34 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3465,7 +3514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3486,6 +3535,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -14263,7 +14324,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B679"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -19719,19 +19780,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A92" sqref="A92:A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -19739,248 +19802,374 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>1081</v>
       </c>
       <c r="B2" s="7">
         <v>33642</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>1082</v>
       </c>
       <c r="B3" s="7">
         <v>34788</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>1083</v>
       </c>
       <c r="B4" s="7">
         <v>33835</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>540</v>
       </c>
       <c r="B5" s="7">
         <v>53510</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>542</v>
       </c>
       <c r="B6" s="7">
         <v>861</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="C6" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>488</v>
       </c>
       <c r="B7" s="7">
         <v>5018</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="C7" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>489</v>
       </c>
       <c r="B8" s="7">
         <v>466</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="C8" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>490</v>
       </c>
       <c r="B9" s="7">
         <v>2852</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="C9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>491</v>
       </c>
       <c r="B10" s="7">
         <v>2344</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="C10" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>492</v>
       </c>
       <c r="B11" s="7">
         <v>2307</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="C11" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>493</v>
       </c>
       <c r="B12" s="7">
         <v>2616</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="C12" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>494</v>
       </c>
       <c r="B13" s="7">
         <v>2896</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="C13" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>495</v>
       </c>
       <c r="B14" s="7">
         <v>2366</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="C14" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>496</v>
       </c>
       <c r="B15" s="7">
         <v>4415</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="C15" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>497</v>
       </c>
       <c r="B16" s="7">
         <v>1910</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="C16" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>498</v>
       </c>
       <c r="B17" s="7">
         <v>8180</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="C17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>499</v>
       </c>
       <c r="B18" s="7">
         <v>2001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="C18" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>1084</v>
       </c>
       <c r="B19" s="7">
         <v>121566</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>543</v>
       </c>
       <c r="B20" s="7">
         <v>6676</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="C20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>1085</v>
       </c>
       <c r="B21" s="7">
         <v>1850</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="C21" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>544</v>
       </c>
       <c r="B22" s="7">
         <v>1544</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="C22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>1086</v>
       </c>
       <c r="B23" s="7">
         <v>3151</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="C23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>545</v>
       </c>
       <c r="B24" s="7">
         <v>1053</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="C24" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>546</v>
       </c>
       <c r="B25" s="7">
         <v>1452</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="C25" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>547</v>
       </c>
       <c r="B26" s="7">
         <v>1640</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="C26" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>1087</v>
       </c>
       <c r="B27" s="7">
         <v>2692</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="C27" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>548</v>
       </c>
       <c r="B28" s="7">
         <v>37910</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>1088</v>
       </c>
       <c r="B29" s="7">
         <v>9088</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>549</v>
       </c>
       <c r="B30" s="7">
         <v>5952</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>1089</v>
       </c>
       <c r="B31" s="7">
         <v>121124</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>1090</v>
       </c>
       <c r="B32" s="7">
@@ -19988,7 +20177,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="11" t="s">
         <v>1091</v>
       </c>
       <c r="B33" s="7">
@@ -19996,7 +20185,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="11" t="s">
         <v>1092</v>
       </c>
       <c r="B34" s="7">
@@ -20004,7 +20193,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
         <v>1093</v>
       </c>
       <c r="B35" s="7">
@@ -20012,7 +20201,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="11" t="s">
         <v>550</v>
       </c>
       <c r="B36" s="7">
@@ -20020,7 +20209,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="11" t="s">
         <v>1094</v>
       </c>
       <c r="B37" s="7">
@@ -20028,7 +20217,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="11" t="s">
         <v>551</v>
       </c>
       <c r="B38" s="7">
@@ -20036,7 +20225,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="11" t="s">
         <v>1095</v>
       </c>
       <c r="B39" s="7">
@@ -20044,7 +20233,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="11" t="s">
         <v>1096</v>
       </c>
       <c r="B40" s="7">
@@ -20052,7 +20241,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="11" t="s">
         <v>1097</v>
       </c>
       <c r="B41" s="7">
@@ -20060,7 +20249,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="11" t="s">
         <v>1098</v>
       </c>
       <c r="B42" s="7">
@@ -20068,7 +20257,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="11" t="s">
         <v>1099</v>
       </c>
       <c r="B43" s="7">
@@ -20076,7 +20265,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="11" t="s">
         <v>552</v>
       </c>
       <c r="B44" s="7">
@@ -20084,7 +20273,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="11" t="s">
         <v>553</v>
       </c>
       <c r="B45" s="7">
@@ -20092,7 +20281,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="11" t="s">
         <v>1100</v>
       </c>
       <c r="B46" s="7">
@@ -20100,7 +20289,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="11" t="s">
         <v>1101</v>
       </c>
       <c r="B47" s="7">
@@ -20108,7 +20297,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="11" t="s">
         <v>1102</v>
       </c>
       <c r="B48" s="7">
@@ -20116,7 +20305,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="11" t="s">
         <v>500</v>
       </c>
       <c r="B49" s="7">
@@ -20124,7 +20313,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="11" t="s">
         <v>501</v>
       </c>
       <c r="B50" s="7">
@@ -20132,7 +20321,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="11" t="s">
         <v>502</v>
       </c>
       <c r="B51" s="7">
@@ -20140,7 +20329,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="11" t="s">
         <v>503</v>
       </c>
       <c r="B52" s="7">
@@ -20148,7 +20337,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="11" t="s">
         <v>504</v>
       </c>
       <c r="B53" s="7">
@@ -20156,7 +20345,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="11" t="s">
         <v>505</v>
       </c>
       <c r="B54" s="7">
@@ -20164,7 +20353,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="11" t="s">
         <v>506</v>
       </c>
       <c r="B55" s="7">
@@ -20172,7 +20361,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="11" t="s">
         <v>507</v>
       </c>
       <c r="B56" s="7">
@@ -20180,7 +20369,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="11" t="s">
         <v>508</v>
       </c>
       <c r="B57" s="7">
@@ -20188,7 +20377,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="11" t="s">
         <v>509</v>
       </c>
       <c r="B58" s="7">
@@ -20196,7 +20385,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="11" t="s">
         <v>510</v>
       </c>
       <c r="B59" s="7">
@@ -20204,7 +20393,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="11" t="s">
         <v>1103</v>
       </c>
       <c r="B60" s="7">
@@ -20212,7 +20401,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="11" t="s">
         <v>1104</v>
       </c>
       <c r="B61" s="7">
@@ -20220,7 +20409,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="11" t="s">
         <v>1105</v>
       </c>
       <c r="B62" s="7">
@@ -20228,7 +20417,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="11" t="s">
         <v>554</v>
       </c>
       <c r="B63" s="7">
@@ -20236,7 +20425,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="11" t="s">
         <v>1106</v>
       </c>
       <c r="B64" s="7">
@@ -20244,7 +20433,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="11" t="s">
         <v>1107</v>
       </c>
       <c r="B65" s="7">
@@ -20252,7 +20441,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="11" t="s">
         <v>1108</v>
       </c>
       <c r="B66" s="7">
@@ -20260,7 +20449,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="11" t="s">
         <v>1109</v>
       </c>
       <c r="B67" s="7">
@@ -20268,7 +20457,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="11" t="s">
         <v>511</v>
       </c>
       <c r="B68" s="7">
@@ -20276,7 +20465,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="11" t="s">
         <v>512</v>
       </c>
       <c r="B69" s="7">
@@ -20284,7 +20473,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="11" t="s">
         <v>513</v>
       </c>
       <c r="B70" s="7">
@@ -20292,7 +20481,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="11" t="s">
         <v>514</v>
       </c>
       <c r="B71" s="7">
@@ -20300,7 +20489,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="11" t="s">
         <v>515</v>
       </c>
       <c r="B72" s="7">
@@ -20308,7 +20497,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="11" t="s">
         <v>516</v>
       </c>
       <c r="B73" s="7">
@@ -20316,7 +20505,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="11" t="s">
         <v>1110</v>
       </c>
       <c r="B74" s="7">
@@ -20324,7 +20513,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="11" t="s">
         <v>1111</v>
       </c>
       <c r="B75" s="7">
@@ -20332,7 +20521,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="11" t="s">
         <v>517</v>
       </c>
       <c r="B76" s="7">
@@ -20340,7 +20529,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="11" t="s">
         <v>1112</v>
       </c>
       <c r="B77" s="7">
@@ -20348,7 +20537,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="11" t="s">
         <v>555</v>
       </c>
       <c r="B78" s="7">
@@ -20356,7 +20545,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="11" t="s">
         <v>1113</v>
       </c>
       <c r="B79" s="7">
@@ -20364,7 +20553,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="11" t="s">
         <v>518</v>
       </c>
       <c r="B80" s="7">
@@ -20372,7 +20561,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="11" t="s">
         <v>519</v>
       </c>
       <c r="B81" s="7">
@@ -20380,7 +20569,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="11" t="s">
         <v>520</v>
       </c>
       <c r="B82" s="7">
@@ -20388,7 +20577,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="11" t="s">
         <v>521</v>
       </c>
       <c r="B83" s="7">
@@ -20396,7 +20585,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="11" t="s">
         <v>522</v>
       </c>
       <c r="B84" s="7">
@@ -20404,7 +20593,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="11" t="s">
         <v>523</v>
       </c>
       <c r="B85" s="7">
@@ -20412,7 +20601,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="11" t="s">
         <v>1114</v>
       </c>
       <c r="B86" s="7">
@@ -20420,7 +20609,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+      <c r="A87" s="11" t="s">
         <v>1115</v>
       </c>
       <c r="B87" s="7">
@@ -20428,7 +20617,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="11" t="s">
         <v>1116</v>
       </c>
       <c r="B88" s="7">
@@ -20436,7 +20625,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="11" t="s">
         <v>1117</v>
       </c>
       <c r="B89" s="7">
@@ -20444,7 +20633,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="11" t="s">
         <v>1118</v>
       </c>
       <c r="B90" s="7">
@@ -20452,7 +20641,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+      <c r="A91" s="11" t="s">
         <v>1119</v>
       </c>
       <c r="B91" s="7">
@@ -20460,7 +20649,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="11" t="s">
         <v>1120</v>
       </c>
       <c r="B92" s="7">
@@ -20468,7 +20657,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="11" t="s">
         <v>1121</v>
       </c>
       <c r="B93" s="7">
@@ -20705,312 +20894,24 @@
       <sortCondition ref="A2:A93"/>
     </sortState>
   </autoFilter>
+  <sortState ref="A2:B149">
+    <sortCondition ref="A2:A149"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C36"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A52" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>490</v>
-      </c>
-      <c r="B3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>491</v>
-      </c>
-      <c r="B4" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>493</v>
-      </c>
-      <c r="B6" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>494</v>
-      </c>
-      <c r="B7" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>495</v>
-      </c>
-      <c r="B8" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>496</v>
-      </c>
-      <c r="B9" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>497</v>
-      </c>
-      <c r="B10" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>498</v>
-      </c>
-      <c r="B11" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>499</v>
-      </c>
-      <c r="B12" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>500</v>
-      </c>
-      <c r="B13" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>501</v>
-      </c>
-      <c r="B14" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>502</v>
-      </c>
-      <c r="B15" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>503</v>
-      </c>
-      <c r="B16" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>504</v>
-      </c>
-      <c r="B17" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>505</v>
-      </c>
-      <c r="B18" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>506</v>
-      </c>
-      <c r="B19" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B20" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>508</v>
-      </c>
-      <c r="B21" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>509</v>
-      </c>
-      <c r="B22" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>510</v>
-      </c>
-      <c r="B23" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>511</v>
-      </c>
-      <c r="B24" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>512</v>
-      </c>
-      <c r="B25" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>513</v>
-      </c>
-      <c r="B26" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>514</v>
-      </c>
-      <c r="B27" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>515</v>
-      </c>
-      <c r="B28" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>516</v>
-      </c>
-      <c r="B29" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>517</v>
-      </c>
-      <c r="B30" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>518</v>
-      </c>
-      <c r="B31" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>519</v>
-      </c>
-      <c r="B32" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>520</v>
-      </c>
-      <c r="B33" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>521</v>
-      </c>
-      <c r="B34" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>522</v>
-      </c>
-      <c r="B35" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>523</v>
-      </c>
-      <c r="B36" t="s">
-        <v>460</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>